<commit_message>
pipelined processor - datapath implementation
</commit_message>
<xml_diff>
--- a/my_single_cycle/instructions.xlsx
+++ b/my_single_cycle/instructions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\my_single_cycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\Heterogeneous-multicore\my_single_cycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A7E49A-6C4D-46D1-A2BC-EA43E8E13A2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F42C7B-B7A2-4E22-9432-588E41CA4368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
   </bookViews>
@@ -399,16 +399,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -417,12 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268BA47F-AF47-4F29-ABE4-FB53CAF89061}">
   <dimension ref="B2:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,21 +754,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -809,7 +809,7 @@
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="16" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="1">
@@ -844,7 +844,7 @@
       <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="1">
@@ -879,7 +879,7 @@
       <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="1">
@@ -914,7 +914,7 @@
       <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="1">
@@ -949,7 +949,7 @@
       <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="16" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="1">
@@ -984,7 +984,7 @@
       <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E9" s="1">
@@ -1013,21 +1013,21 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1051,20 +1051,20 @@
       <c r="I12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18" t="s">
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18" t="s">
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="Q12" s="18"/>
+      <c r="Q12" s="19"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
@@ -1091,20 +1091,20 @@
       <c r="I13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17" t="s">
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17" t="s">
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Q13" s="17"/>
+      <c r="Q13" s="18"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
@@ -1113,14 +1113,14 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
@@ -1136,25 +1136,25 @@
       <c r="F15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18" t="s">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18" t="s">
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18" t="s">
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="Q15" s="18"/>
+      <c r="Q15" s="19"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
@@ -1163,7 +1163,7 @@
       <c r="C16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="16" t="s">
         <v>62</v>
       </c>
       <c r="E16" s="13" t="s">
@@ -1172,25 +1172,25 @@
       <c r="F16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17" t="s">
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17" t="s">
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="17"/>
+      <c r="Q16" s="18"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
@@ -1199,7 +1199,7 @@
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="13" t="s">
@@ -1208,25 +1208,25 @@
       <c r="F17" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17" t="s">
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17" t="s">
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17" t="s">
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="Q17" s="17"/>
+      <c r="Q17" s="18"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
@@ -1235,7 +1235,7 @@
       <c r="C18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="13" t="s">
@@ -1244,25 +1244,25 @@
       <c r="F18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17" t="s">
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17" t="s">
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17" t="s">
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="17"/>
+      <c r="Q18" s="18"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
@@ -1271,7 +1271,7 @@
       <c r="C19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="16" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="13" t="s">
@@ -1280,36 +1280,36 @@
       <c r="F19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17" t="s">
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17" t="s">
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17" t="s">
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="Q19" s="17"/>
+      <c r="Q19" s="18"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -1319,27 +1319,27 @@
       <c r="D21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18" t="s">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18" t="s">
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18" t="s">
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="Q21" s="18"/>
+      <c r="Q21" s="19"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
@@ -1348,38 +1348,38 @@
       <c r="C22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17" t="s">
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17" t="s">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N22" s="17"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="19" t="s">
+      <c r="N22" s="18"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="19"/>
+      <c r="Q22" s="23"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="10" t="s">
@@ -1442,16 +1442,21 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="P22:Q23"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="M13:O13"/>
@@ -1468,22 +1473,17 @@
     <mergeCell ref="J19:L19"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="J21:L21"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
     <mergeCell ref="C11:L11"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="P22:Q23"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
execution and writeback stages written
</commit_message>
<xml_diff>
--- a/my_single_cycle/instructions.xlsx
+++ b/my_single_cycle/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\Heterogeneous-multicore\my_single_cycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F42C7B-B7A2-4E22-9432-588E41CA4368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECEC87-DF57-446E-B8EE-DEC457D6D98A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
   </bookViews>
@@ -408,6 +408,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,12 +421,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -739,13 +739,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268BA47F-AF47-4F29-ABE4-FB53CAF89061}">
   <dimension ref="B2:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
@@ -754,18 +754,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
@@ -1013,18 +1013,18 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -1113,14 +1113,14 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
@@ -1302,14 +1302,14 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -1367,16 +1367,16 @@
         <v>51</v>
       </c>
       <c r="N22" s="18"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="23" t="s">
+      <c r="O22" s="21"/>
+      <c r="P22" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="23"/>
+      <c r="Q22" s="20"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C25" s="15" t="s">
@@ -1442,6 +1442,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="E22:I22"/>
@@ -1458,32 +1484,6 @@
     <mergeCell ref="P19:Q19"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the repo with some docs - added 5 stage pipeline diagram
</commit_message>
<xml_diff>
--- a/my_single_cycle/instructions.xlsx
+++ b/my_single_cycle/instructions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\Heterogeneous-multicore\my_single_cycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NCSU_classes_files\spring20\633\Project\Heterogeneous-multicore\my_5_stage_proc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECEC87-DF57-446E-B8EE-DEC457D6D98A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE21AC7-3672-415F-B7D0-A6FAA92531C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="369" activeTab="1" xr2:uid="{718E7806-298C-4F07-8385-55875B93F518}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="143">
   <si>
     <t>RTYPE</t>
   </si>
@@ -240,6 +241,228 @@
   </si>
   <si>
     <t>intsn count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addi $2 $0 5          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">addi $3 $0 12         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">addi $7 $3 -9         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">or $4 $7 $2           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">and $5 $3 $4          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add $5 $5 $4          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">beq $5 $7 &gt;end        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">slt $4 $3 $4          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">beq $4 $0 &gt;around     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">addi $5 $0 0          </t>
+  </si>
+  <si>
+    <t>slt $4 $7 $2   &lt;around</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add $7 $4 $5          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub $7 $7 $2          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw $7 68 ($3)         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lw $2 80 ($0)         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j &gt;end                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">addi $2 $0 1          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw $2 84 ($0)   &lt;end  </t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># initialize $2 = 5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># initialize $3 = 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># initialize $7 = 3  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $4 = (3 OR 5) = 7  </t>
+  </si>
+  <si>
+    <t># $5 = (12 AND 7) = 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $5 = 4 + 7 = 11    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># shouldn’t be taken </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $4 = 12 &lt; 7 = 0    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># should be taken    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># shouldn’t happen   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $4 = 3 &lt; 5 = 1     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $7 = 1 + 11 = 12   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $7 = 12 − 5 = 7    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># [80] = 7           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># $2 = [80] = 7      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># shouldn't happen   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"># write mem[84] = 7  </t>
+  </si>
+  <si>
+    <t>Instn Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c </t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>0x20020005</t>
+  </si>
+  <si>
+    <t>0x2003000c</t>
+  </si>
+  <si>
+    <t>0x2067fff7</t>
+  </si>
+  <si>
+    <t>0x00e22025</t>
+  </si>
+  <si>
+    <t>0x00642824</t>
+  </si>
+  <si>
+    <t>0x00a42820</t>
+  </si>
+  <si>
+    <t>0x10a7000a</t>
+  </si>
+  <si>
+    <t>0x0064202a</t>
+  </si>
+  <si>
+    <t>0x10800001</t>
+  </si>
+  <si>
+    <t>0x20050000</t>
+  </si>
+  <si>
+    <t>0x00e2202a</t>
+  </si>
+  <si>
+    <t>0x00853820</t>
+  </si>
+  <si>
+    <t>0x00e23822</t>
+  </si>
+  <si>
+    <t>0xac670044</t>
+  </si>
+  <si>
+    <t>0x8c020050</t>
+  </si>
+  <si>
+    <t>0x08000011</t>
+  </si>
+  <si>
+    <t>0x20020001</t>
+  </si>
+  <si>
+    <t>0xac020054</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F </t>
+  </si>
+  <si>
+    <t>Optional Instructions</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>32'b0</t>
+  </si>
+  <si>
+    <t>32'hFC000000</t>
+  </si>
+  <si>
+    <t>squash</t>
   </si>
 </sst>
 </file>
@@ -275,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +526,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,16 +631,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -423,6 +656,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,15 +977,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268BA47F-AF47-4F29-ABE4-FB53CAF89061}">
-  <dimension ref="B2:Q30"/>
+  <dimension ref="B2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
@@ -754,18 +994,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
@@ -1013,18 +1253,18 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -1051,20 +1291,20 @@
       <c r="I12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19" t="s">
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19" t="s">
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="Q12" s="19"/>
+      <c r="Q12" s="25"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
@@ -1091,20 +1331,20 @@
       <c r="I13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18" t="s">
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18" t="s">
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="Q13" s="18"/>
+      <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
@@ -1113,14 +1353,14 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
@@ -1136,25 +1376,25 @@
       <c r="F15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19" t="s">
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19" t="s">
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19" t="s">
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="Q15" s="19"/>
+      <c r="Q15" s="25"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
@@ -1172,25 +1412,25 @@
       <c r="F16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18" t="s">
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18" t="s">
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18" t="s">
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="18"/>
+      <c r="Q16" s="24"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
@@ -1208,25 +1448,25 @@
       <c r="F17" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18" t="s">
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18" t="s">
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18" t="s">
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="Q17" s="18"/>
+      <c r="Q17" s="24"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
@@ -1244,25 +1484,25 @@
       <c r="F18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18" t="s">
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18" t="s">
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18" t="s">
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="18"/>
+      <c r="Q18" s="24"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
@@ -1280,36 +1520,36 @@
       <c r="F19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18" t="s">
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18" t="s">
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18" t="s">
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="Q19" s="18"/>
+      <c r="Q19" s="24"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -1319,27 +1559,27 @@
       <c r="D21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19" t="s">
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19" t="s">
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19" t="s">
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="Q21" s="19"/>
+      <c r="Q21" s="25"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
@@ -1351,108 +1591,139 @@
       <c r="D22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18" t="s">
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18" t="s">
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="N22" s="18"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="20" t="s">
+      <c r="N22" s="24"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="20"/>
+      <c r="Q22" s="29"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="2">
-        <v>100010</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="2">
-        <v>100100</v>
-      </c>
+      <c r="C28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="2">
-        <v>100101</v>
+        <v>100000</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="2">
+        <v>100010</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="2">
+        <v>100100</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="2">
+        <v>100101</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D33" s="2">
         <v>101010</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="P22:Q23"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="M13:O13"/>
     <mergeCell ref="M14:O14"/>
@@ -1469,24 +1740,725 @@
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="M19:O19"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="P22:Q23"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC80CC1-2568-45BC-8C8F-5C49C714F2FC}">
+  <dimension ref="A4:AE22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="21">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
+        <v>2</v>
+      </c>
+      <c r="H4" s="21">
+        <v>3</v>
+      </c>
+      <c r="I4" s="21">
+        <v>4</v>
+      </c>
+      <c r="J4" s="21">
+        <v>5</v>
+      </c>
+      <c r="K4" s="21">
+        <v>6</v>
+      </c>
+      <c r="L4" s="21">
+        <v>7</v>
+      </c>
+      <c r="M4" s="21">
+        <v>8</v>
+      </c>
+      <c r="N4" s="21">
+        <v>9</v>
+      </c>
+      <c r="O4" s="21">
+        <v>10</v>
+      </c>
+      <c r="P4" s="21">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>12</v>
+      </c>
+      <c r="R4" s="21">
+        <v>13</v>
+      </c>
+      <c r="S4" s="21">
+        <v>14</v>
+      </c>
+      <c r="T4" s="21">
+        <v>15</v>
+      </c>
+      <c r="U4" s="21">
+        <v>16</v>
+      </c>
+      <c r="V4" s="21">
+        <v>17</v>
+      </c>
+      <c r="W4" s="21">
+        <v>18</v>
+      </c>
+      <c r="X4" s="21">
+        <v>19</v>
+      </c>
+      <c r="Y4" s="21">
+        <v>20</v>
+      </c>
+      <c r="Z4" s="21">
+        <v>21</v>
+      </c>
+      <c r="AA4" s="21">
+        <v>22</v>
+      </c>
+      <c r="AB4" s="21">
+        <v>23</v>
+      </c>
+      <c r="AC4" s="21">
+        <v>24</v>
+      </c>
+      <c r="AD4" s="21">
+        <v>25</v>
+      </c>
+      <c r="AE4" s="21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="18">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="18">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" t="s">
+        <v>133</v>
+      </c>
+      <c r="L8" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="18">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" t="s">
+        <v>132</v>
+      </c>
+      <c r="L9" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="18">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M10" t="s">
+        <v>133</v>
+      </c>
+      <c r="N10" t="s">
+        <v>134</v>
+      </c>
+      <c r="O10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="18">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L11" t="s">
+        <v>131</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="N11" t="s">
+        <v>132</v>
+      </c>
+      <c r="O11" t="s">
+        <v>133</v>
+      </c>
+      <c r="P11" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="N12" t="s">
+        <v>131</v>
+      </c>
+      <c r="O12" t="s">
+        <v>132</v>
+      </c>
+      <c r="P12" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="18">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+      <c r="O13" t="s">
+        <v>131</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>132</v>
+      </c>
+      <c r="R13" t="s">
+        <v>133</v>
+      </c>
+      <c r="S13" t="s">
+        <v>134</v>
+      </c>
+      <c r="T13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="18">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q14" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="R14" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="S14" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="T14" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="U14" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="18">
+        <v>28</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="R15" t="s">
+        <v>131</v>
+      </c>
+      <c r="S15" t="s">
+        <v>132</v>
+      </c>
+      <c r="T15" t="s">
+        <v>133</v>
+      </c>
+      <c r="U15" t="s">
+        <v>134</v>
+      </c>
+      <c r="V15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>124</v>
+      </c>
+      <c r="S16" t="s">
+        <v>131</v>
+      </c>
+      <c r="T16" t="s">
+        <v>132</v>
+      </c>
+      <c r="U16" t="s">
+        <v>133</v>
+      </c>
+      <c r="V16" t="s">
+        <v>134</v>
+      </c>
+      <c r="W16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="18">
+        <v>30</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="T17" t="s">
+        <v>131</v>
+      </c>
+      <c r="U17" t="s">
+        <v>132</v>
+      </c>
+      <c r="V17" t="s">
+        <v>133</v>
+      </c>
+      <c r="W17" t="s">
+        <v>134</v>
+      </c>
+      <c r="X17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="18">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="U18" t="s">
+        <v>131</v>
+      </c>
+      <c r="V18" t="s">
+        <v>132</v>
+      </c>
+      <c r="W18" t="s">
+        <v>133</v>
+      </c>
+      <c r="X18" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="18">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>127</v>
+      </c>
+      <c r="V19" t="s">
+        <v>131</v>
+      </c>
+      <c r="W19" t="s">
+        <v>132</v>
+      </c>
+      <c r="X19" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
+      <c r="W20" t="s">
+        <v>131</v>
+      </c>
+      <c r="X20" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="18">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>129</v>
+      </c>
+      <c r="X21" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y21" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="18">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>